<commit_message>
Tabelas de serviço, categoria atualizadas
tabelas atualizadas
</commit_message>
<xml_diff>
--- a/documentacao/DB/Tabelas de serviço, categoria e relação serviço-categoria.xlsx
+++ b/documentacao/DB/Tabelas de serviço, categoria e relação serviço-categoria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luciana\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E635BD5-6107-450E-ACAE-0880225C2918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272A1EA4-E3F0-491F-AA60-3C13A8C41384}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{65EF6087-825B-4F3A-B834-03C4183BBCBB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>CATEGORIA</t>
   </si>
@@ -50,13 +50,7 @@
     <t>Servico</t>
   </si>
   <si>
-    <t>rl_categoria_servico</t>
-  </si>
-  <si>
     <t>fk_categoria</t>
-  </si>
-  <si>
-    <t>fk_servico</t>
   </si>
   <si>
     <t>HIDRÁULICA</t>
@@ -189,17 +183,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -234,7 +220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -275,6 +261,17 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -291,16 +288,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -617,551 +614,454 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C9C396-A43E-44E4-AA0D-ACCA99DAF643}">
-  <dimension ref="A2:H33"/>
+  <dimension ref="A2:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="5"/>
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="G2" s="5" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="1">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1">
         <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="1">
-        <v>2</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1">
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="1">
-        <v>2</v>
-      </c>
-      <c r="H8" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="F8" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1">
         <v>6</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="1">
-        <v>2</v>
-      </c>
-      <c r="H9" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1">
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="1">
-        <v>2</v>
-      </c>
-      <c r="H10" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1">
         <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="1">
-        <v>3</v>
-      </c>
-      <c r="H11" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1">
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="1">
-        <v>3</v>
-      </c>
-      <c r="H12" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D13" s="1">
         <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="1">
+        <v>27</v>
+      </c>
+      <c r="F13" s="1">
         <v>4</v>
       </c>
-      <c r="H13" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1">
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="1">
-        <v>4</v>
-      </c>
-      <c r="H14" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1">
         <v>12</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="1">
-        <v>4</v>
-      </c>
-      <c r="H15" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
         <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="1">
-        <v>5</v>
-      </c>
-      <c r="H16" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="F16" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
         <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="1">
-        <v>5</v>
-      </c>
-      <c r="H17" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="F17" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="1">
-        <v>6</v>
-      </c>
-      <c r="H18" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <v>16</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="1">
-        <v>6</v>
-      </c>
-      <c r="H19" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="F19" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <v>17</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="1">
-        <v>6</v>
-      </c>
-      <c r="H20" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="F20" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>18</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="1">
+        <v>35</v>
+      </c>
+      <c r="F21" s="1">
         <v>7</v>
       </c>
-      <c r="H21" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <v>19</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="1">
+        <v>36</v>
+      </c>
+      <c r="F22" s="1">
         <v>7</v>
       </c>
-      <c r="H22" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <v>20</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23" s="1">
+        <v>37</v>
+      </c>
+      <c r="F23" s="1">
         <v>7</v>
       </c>
-      <c r="H23" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D24" s="1">
         <v>21</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G24" s="1">
+        <v>38</v>
+      </c>
+      <c r="F24" s="1">
         <v>7</v>
       </c>
-      <c r="H24" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
         <v>22</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G25" s="1">
+        <v>39</v>
+      </c>
+      <c r="F25" s="1">
         <v>7</v>
       </c>
-      <c r="H25" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
         <v>23</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G26" s="1">
+        <v>40</v>
+      </c>
+      <c r="F26" s="1">
         <v>7</v>
       </c>
-      <c r="H26" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <v>24</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G27" s="1">
+        <v>41</v>
+      </c>
+      <c r="F27" s="1">
         <v>7</v>
       </c>
-      <c r="H27" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D28" s="1">
         <v>25</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G28" s="1">
-        <v>8</v>
-      </c>
-      <c r="H28" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D29" s="1">
         <v>26</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G29" s="1">
-        <v>9</v>
-      </c>
-      <c r="H29" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D30" s="1">
         <v>27</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G30" s="1">
-        <v>10</v>
-      </c>
-      <c r="H30" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="F30" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D31" s="1">
         <v>28</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G31" s="1">
-        <v>10</v>
-      </c>
-      <c r="H31" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F31" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D32" s="1">
         <v>29</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G32" s="1">
-        <v>11</v>
-      </c>
-      <c r="H32" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F32" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <v>30</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G33" s="1">
-        <v>12</v>
-      </c>
-      <c r="H33" s="1">
-        <v>14</v>
+        <v>47</v>
+      </c>
+      <c r="F33" s="1">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="D2:F2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>